<commit_message>
Se agregó un manejo de error en el archivo test.ipynb para capturar el error de módulo no encontrado para 'pandas'. Se actualizaron los archivos de caché y se modificó el archivo de Excel MontosMotoboy_sushi_club.xlsx.
</commit_message>
<xml_diff>
--- a/exports/MontosMotoboy_sushi_club.xlsx
+++ b/exports/MontosMotoboy_sushi_club.xlsx
@@ -487,25 +487,25 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4330</v>
+        <v>4637</v>
       </c>
       <c r="C2" t="n">
-        <v>4330</v>
+        <v>4637</v>
       </c>
       <c r="D2" t="n">
-        <v>4363</v>
+        <v>4631</v>
       </c>
       <c r="E2" t="n">
-        <v>4613</v>
+        <v>4896</v>
       </c>
       <c r="F2" t="n">
-        <v>4613</v>
+        <v>4896</v>
       </c>
       <c r="G2" t="n">
-        <v>4422</v>
+        <v>4539</v>
       </c>
       <c r="H2" t="n">
-        <v>4224</v>
+        <v>4485</v>
       </c>
       <c r="I2" t="n">
         <v>4613</v>
@@ -518,25 +518,25 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3936</v>
+        <v>4216</v>
       </c>
       <c r="C3" t="n">
-        <v>3936</v>
+        <v>4216</v>
       </c>
       <c r="D3" t="n">
-        <v>3966</v>
+        <v>4210</v>
       </c>
       <c r="E3" t="n">
-        <v>4194</v>
+        <v>4451</v>
       </c>
       <c r="F3" t="n">
-        <v>4194</v>
+        <v>4451</v>
       </c>
       <c r="G3" t="n">
-        <v>4020</v>
+        <v>4127</v>
       </c>
       <c r="H3" t="n">
-        <v>3840</v>
+        <v>4078</v>
       </c>
       <c r="I3" t="n">
         <v>4194</v>
@@ -549,25 +549,25 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4330</v>
+        <v>4637</v>
       </c>
       <c r="C4" t="n">
-        <v>4330</v>
+        <v>4637</v>
       </c>
       <c r="D4" t="n">
-        <v>4363</v>
+        <v>4631</v>
       </c>
       <c r="E4" t="n">
-        <v>4613</v>
+        <v>4896</v>
       </c>
       <c r="F4" t="n">
-        <v>4613</v>
+        <v>4896</v>
       </c>
       <c r="G4" t="n">
-        <v>4422</v>
+        <v>4539</v>
       </c>
       <c r="H4" t="n">
-        <v>4224</v>
+        <v>4485</v>
       </c>
       <c r="I4" t="n">
         <v>4613</v>
@@ -580,25 +580,25 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3936</v>
+        <v>4216</v>
       </c>
       <c r="C5" t="n">
-        <v>3936</v>
+        <v>4216</v>
       </c>
       <c r="D5" t="n">
-        <v>3966</v>
+        <v>4210</v>
       </c>
       <c r="E5" t="n">
-        <v>4194</v>
+        <v>4451</v>
       </c>
       <c r="F5" t="n">
-        <v>4194</v>
+        <v>4451</v>
       </c>
       <c r="G5" t="n">
-        <v>4020</v>
+        <v>4127</v>
       </c>
       <c r="H5" t="n">
-        <v>3840</v>
+        <v>4078</v>
       </c>
       <c r="I5" t="n">
         <v>4194</v>
@@ -611,25 +611,25 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>5148</v>
+        <v>5465</v>
       </c>
       <c r="C6" t="n">
-        <v>5148</v>
+        <v>5465</v>
       </c>
       <c r="D6" t="n">
-        <v>4932</v>
+        <v>5237</v>
       </c>
       <c r="E6" t="n">
-        <v>5076</v>
+        <v>5444</v>
       </c>
       <c r="F6" t="n">
-        <v>5076</v>
+        <v>5444</v>
       </c>
       <c r="G6" t="n">
-        <v>5790</v>
+        <v>6162</v>
       </c>
       <c r="H6" t="n">
-        <v>5406</v>
+        <v>5741</v>
       </c>
       <c r="I6" t="n">
         <v>5784</v>
@@ -642,25 +642,25 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>4794</v>
+        <v>5093</v>
       </c>
       <c r="C7" t="n">
-        <v>4794</v>
+        <v>5093</v>
       </c>
       <c r="D7" t="n">
-        <v>4638</v>
+        <v>4927</v>
       </c>
       <c r="E7" t="n">
-        <v>4692</v>
+        <v>5065</v>
       </c>
       <c r="F7" t="n">
-        <v>4692</v>
+        <v>5065</v>
       </c>
       <c r="G7" t="n">
-        <v>5346</v>
+        <v>5693</v>
       </c>
       <c r="H7" t="n">
-        <v>5010</v>
+        <v>5320</v>
       </c>
       <c r="I7" t="n">
         <v>5364</v>
@@ -673,25 +673,25 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>4338</v>
+        <v>4602</v>
       </c>
       <c r="C8" t="n">
-        <v>4338</v>
+        <v>4602</v>
       </c>
       <c r="D8" t="n">
-        <v>4146</v>
+        <v>4403</v>
       </c>
       <c r="E8" t="n">
-        <v>4260</v>
+        <v>4589</v>
       </c>
       <c r="F8" t="n">
-        <v>4260</v>
+        <v>4589</v>
       </c>
       <c r="G8" t="n">
-        <v>5028</v>
+        <v>5354</v>
       </c>
       <c r="H8" t="n">
-        <v>4536</v>
+        <v>4817</v>
       </c>
       <c r="I8" t="n">
         <v>5052</v>
@@ -704,25 +704,25 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>4146</v>
+        <v>4403</v>
       </c>
       <c r="C9" t="n">
-        <v>4146</v>
+        <v>4403</v>
       </c>
       <c r="D9" t="n">
-        <v>3906</v>
+        <v>4147</v>
       </c>
       <c r="E9" t="n">
-        <v>3930</v>
+        <v>4210</v>
       </c>
       <c r="F9" t="n">
-        <v>3930</v>
+        <v>4210</v>
       </c>
       <c r="G9" t="n">
-        <v>4782</v>
+        <v>5093</v>
       </c>
       <c r="H9" t="n">
-        <v>4380</v>
+        <v>4651</v>
       </c>
       <c r="I9" t="n">
         <v>4728</v>
@@ -735,25 +735,25 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>6402</v>
+        <v>6797</v>
       </c>
       <c r="C10" t="n">
-        <v>6402</v>
+        <v>6797</v>
       </c>
       <c r="D10" t="n">
-        <v>6126</v>
+        <v>6506</v>
       </c>
       <c r="E10" t="n">
-        <v>6450</v>
+        <v>6914</v>
       </c>
       <c r="F10" t="n">
-        <v>6450</v>
+        <v>6914</v>
       </c>
       <c r="G10" t="n">
-        <v>7326</v>
+        <v>7804</v>
       </c>
       <c r="H10" t="n">
-        <v>6696</v>
+        <v>7114</v>
       </c>
       <c r="I10" t="n">
         <v>7224</v>
@@ -766,25 +766,25 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>5958</v>
+        <v>6328</v>
       </c>
       <c r="C11" t="n">
-        <v>5958</v>
+        <v>6328</v>
       </c>
       <c r="D11" t="n">
-        <v>5778</v>
+        <v>6134</v>
       </c>
       <c r="E11" t="n">
-        <v>6072</v>
+        <v>6506</v>
       </c>
       <c r="F11" t="n">
-        <v>6072</v>
+        <v>6506</v>
       </c>
       <c r="G11" t="n">
-        <v>6822</v>
+        <v>7146</v>
       </c>
       <c r="H11" t="n">
-        <v>6240</v>
+        <v>6624</v>
       </c>
       <c r="I11" t="n">
         <v>6762</v>
@@ -797,25 +797,25 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>5334</v>
+        <v>5665</v>
       </c>
       <c r="C12" t="n">
-        <v>5334</v>
+        <v>5665</v>
       </c>
       <c r="D12" t="n">
-        <v>5250</v>
+        <v>5575</v>
       </c>
       <c r="E12" t="n">
-        <v>5544</v>
+        <v>5941</v>
       </c>
       <c r="F12" t="n">
-        <v>5544</v>
+        <v>5941</v>
       </c>
       <c r="G12" t="n">
-        <v>6282</v>
+        <v>6686</v>
       </c>
       <c r="H12" t="n">
-        <v>5592</v>
+        <v>5941</v>
       </c>
       <c r="I12" t="n">
         <v>6102</v>
@@ -828,25 +828,25 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>5178</v>
+        <v>5500</v>
       </c>
       <c r="C13" t="n">
-        <v>5178</v>
+        <v>5500</v>
       </c>
       <c r="D13" t="n">
-        <v>5016</v>
+        <v>5327</v>
       </c>
       <c r="E13" t="n">
-        <v>5214</v>
+        <v>5590</v>
       </c>
       <c r="F13" t="n">
-        <v>5214</v>
+        <v>5590</v>
       </c>
       <c r="G13" t="n">
-        <v>5874</v>
+        <v>6252</v>
       </c>
       <c r="H13" t="n">
-        <v>5424</v>
+        <v>5761</v>
       </c>
       <c r="I13" t="n">
         <v>5886</v>

</xml_diff>